<commit_message>
FHIR profiles per Oncology implementation guide
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-oncology-kenya-condition.xlsx
+++ b/output/StructureDefinition-oncology-kenya-condition.xlsx
@@ -45,13 +45,13 @@
     <t>Title</t>
   </si>
   <si>
-    <t>oncology kenya condition</t>
+    <t>Oncology Kenya Condition</t>
   </si>
   <si>
     <t>Status</t>
   </si>
   <si>
-    <t>draft</t>
+    <t>active</t>
   </si>
   <si>
     <t>Experimental</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-06-10T13:49:52+03:00</t>
+    <t>2025-06-30T18:02:10+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -84,7 +84,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>condition profile from oncology diagnoses in Kenya, ensuring structured documentation and national cancer registry reporting.</t>
+    <t>A Condition profile for structured oncology diagnosis documentation in Kenya, aligned with national cancer registry reporting and HL7® FHIR® standards.</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -509,10 +509,10 @@
 </t>
   </si>
   <si>
-    <t>active | recurrence | relapse | inactive | remission | resolved</t>
-  </si>
-  <si>
-    <t>The clinical status of the condition.</t>
+    <t>Active, recurrence, remission, resolved</t>
+  </si>
+  <si>
+    <t>The clinical status of the condition, required for longitudinal tracking and outcomes.</t>
   </si>
   <si>
     <t>The data type is CodeableConcept because clinicalStatus has some clinical judgment involved, such that there might need to be more specificity than the required FHIR value set allows. For example, a SNOMED coding might allow for additional specificity.</t>
@@ -583,10 +583,10 @@
     <t>Condition.category</t>
   </si>
   <si>
-    <t>problem-list-item | encounter-diagnosis</t>
-  </si>
-  <si>
-    <t>A category assigned to the condition.</t>
+    <t>Kenya-specific condition categories</t>
+  </si>
+  <si>
+    <t>Clinical grouping of condition as defined in Kenyan clinical policy or registry definitions.</t>
   </si>
   <si>
     <t>The categorization is often highly contextual and may appear poorly differentiated or not very useful in other contexts.</t>
@@ -613,10 +613,10 @@
     <t>Condition.severity</t>
   </si>
   <si>
-    <t>Subjective severity of condition</t>
-  </si>
-  <si>
-    <t>A subjective assessment of the severity of the condition as evaluated by the clinician.</t>
+    <t>Severity level (e.g., mild, moderate, severe)</t>
+  </si>
+  <si>
+    <t>Clinical severity of the cancer at diagnosis or during follow-up.</t>
   </si>
   <si>
     <t>Coding of the severity with a terminology is preferred, where possible.</t>
@@ -647,10 +647,10 @@
 </t>
   </si>
   <si>
-    <t>Identification of the condition, problem or diagnosis</t>
-  </si>
-  <si>
-    <t>Identification of the condition, problem or diagnosis.</t>
+    <t>ICD-10 diagnosis code</t>
+  </si>
+  <si>
+    <t>Diagnosis code for oncology condition using ICD-10 classification.</t>
   </si>
   <si>
     <t>0..1 to account for primarily narrative only resources.</t>
@@ -783,10 +783,10 @@
 AgePeriodRangestring</t>
   </si>
   <si>
-    <t>Estimated or actual date,  date-time, or age</t>
-  </si>
-  <si>
-    <t>Estimated or actual date or date-time  the condition began, in the opinion of the clinician.</t>
+    <t>Onset date/time or period</t>
+  </si>
+  <si>
+    <t>Mandatory onset information for surveillance and clinical relevance.</t>
   </si>
   <si>
     <t>Age is generally used when the patient reports an age at which the Condition began to occur.</t>
@@ -833,10 +833,10 @@
 </t>
   </si>
   <si>
-    <t>Date record was first recorded</t>
-  </si>
-  <si>
-    <t>The recordedDate represents when this particular Condition record was created in the system, which is often a system-generated date.</t>
+    <t>Date of documentation</t>
+  </si>
+  <si>
+    <t>The date the condition was first recorded in the system.</t>
   </si>
   <si>
     <t>REL-11</t>
@@ -2807,13 +2807,13 @@
       </c>
       <c r="E12" s="2"/>
       <c r="F12" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="G12" t="s" s="2">
         <v>90</v>
       </c>
       <c r="H12" t="s" s="2">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="I12" t="s" s="2">
         <v>91</v>
@@ -3051,7 +3051,7 @@
         <v>80</v>
       </c>
       <c r="H14" t="s" s="2">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="I14" t="s" s="2">
         <v>20</v>
@@ -3169,7 +3169,7 @@
         <v>90</v>
       </c>
       <c r="H15" t="s" s="2">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="I15" t="s" s="2">
         <v>20</v>
@@ -3281,13 +3281,13 @@
       </c>
       <c r="E16" s="2"/>
       <c r="F16" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="G16" t="s" s="2">
         <v>90</v>
       </c>
       <c r="H16" t="s" s="2">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="I16" t="s" s="2">
         <v>20</v>

</xml_diff>